<commit_message>
final: everything is controlled
</commit_message>
<xml_diff>
--- a/output/common_words/xls/common_words_among_websites_dict.xlsx
+++ b/output/common_words/xls/common_words_among_websites_dict.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,60 +453,570 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>Cookies</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://www.yyy.at/ (54), https://www.xxx.at/ (6), https://www.zzz.at/ (11)</t>
+          <t>https://www.100-dakar.com (14), https://www.benjaminwahl.at (18), https://www.dasholzhaus.at (11), https://www.diequote.at (24), https://www.drehorgelkabarett.at (14), https://www.frautomani.at (4), https://www.ingridschiller.at (14), https://www.ottosaxinger.at (3), https://www.peligro.at (14), https://www.reinhardreisenzahn.com (4), https://www.schuledesungehorsams.at (2), https://www.skodone.at (18)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>Linz</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>68</v>
+        <v>330</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://www.yyy.at/ (52), https://www.xxx.at/ (6), https://www.zzz.at/ (10)</t>
+          <t>https://www.die-schule.at (91), https://www.finopoly.at (5), https://www.freie-medien.at (10), https://www.freizeitundkommunikation.at (3), https://www.linzfmr.at (18), https://www.pflueckt.at (3), https://www.qujochoe.org (174), https://www.steingeschichten.at (21), https://www.velodrom-linz.at (5)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>Film</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://www.yyy.at/ (50), https://www.xxx.at/ (5)</t>
+          <t>https://www.apileofghosts.com (16), https://www.boxafilm.com (8), https://www.corpushomini.info (3), https://www.doublehappiness.at (12), https://www.hauntedspaces.net (5), https://www.retrogoldmine.com (8)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>D2</t>
+          <t>Art</t>
         </is>
       </c>
       <c r="B5" t="n">
+        <v>45</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.eipcp.net (13), https://www.faces-l.net (16), https://www.kairus.org (6), https://www.negentropy-sport.net (2), https://www.radical-openness.org (8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Website</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>36</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.apephonie.org (2), https://www.dasholzhaus.at (10), https://www.drehorgelkabarett.at (8), https://www.ingridschiller.at (8), https://www.peligro.at (8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Page</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>35</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.hungaromedia.at (8), https://www.kuenstlerinnen.at (8), https://www.luckeneder-art.at (8), https://www.platform-socialism.org (3), https://www.regional-express.org (8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Mehr</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>95</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.derschueler.at (4), https://www.diebresche.org (23), https://www.lotta-gaffa.at (3), https://www.programmkinowels.at (65)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>März</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>49</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.das-kollektiv.at (8), https://www.feminismus-krawall.at (16), https://www.fiftitu.at (19), https://www.unkraut-comics.at (6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Rocky</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>32</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.hungaromedia.at (8), https://www.kuenstlerinnen.at (8), https://www.luckeneder-art.at (8), https://www.regional-express.org (8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Schule</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>294</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.alteschule-gutau.at (4), https://www.derschueler.at (5), https://www.die-schule.at (285)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Uhr</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>202</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.fro.at (20), https://www.qujochoe.org (170), https://www.rudolfhabringer.at (12)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Radio</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>177</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.radio-fri.at (6), https://www.schulradiotag.at (169), https://www.wegstrecken.at (2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Theater</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>65</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://www.remorauscher.at (41), https://www.theater-tamtam.org (5), https://www.theaternacht.at (19)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Kultur</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>34</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://www.frauenkultur.at (17), https://www.igkultur.at (14), https://www.konsortium.at (3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Kunst</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>26</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://www.frauenkultur.at (16), https://www.kupf.at (6), https://www.triviale.at (4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Festival</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>21</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://www.apileofghosts.com (11), https://www.filmriss.at (5), https://www.radical-openness.org (5)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Arbeiten</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>14</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://www.apephonie.org (2), https://www.fiftitu.at (10), https://www.leodressel.net (2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Site</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
         <v>13</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>https://www.xxx.at/ (5), https://www.zzz.at/ (8)</t>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://www.benjaminwahl.at (5), https://www.downinthehole.org (3), https://www.skodone.at (5)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>45</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://www.archivia.at (33), https://www.rotespuren.at (12)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Music</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://www.lauthals.org (16), https://www.totalsilence.de (4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Menschen</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>18</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://www.donau-danube.eu (3), https://www.vonunten.at (15)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Bürgerinnenrat</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>23</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://www.buergerinnenrat.at (8), https://www.vonunten.at (15)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Work</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>18</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://www.eliot.at (7), https://www.grgr.at (11)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Read</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>17</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://www.ellaraidel.com (7), https://www.freie-medien.at (10)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Magdalena</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>12</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://www.magdalenareiter.at (2), https://www.themagdalenaproject.org (10)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>20</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://www.anna-fiala.at (10), https://www.graztermine.at (10)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Labor</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>10</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://www.hoerstadt.at (2), https://www.migrazine.at (8)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Verein</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>10</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://www.hr-ctrl.or.at (3), https://www.verein-ent.at (7)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>One</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>9</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://www.arttraffic-strand.net (2), https://www.bb15.at (7)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>View</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>12</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://www.boxafilm.com (6), https://www.retrogoldmine.com (6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Speicherung</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>12</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://www.radio-fri.at (6), https://www.theater-tamtam.org (6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Februar</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>12</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://www.tabeacray.com (6), https://www.unkraut-comics.at (6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Andreas</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>8</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://www.andreaskurz.net (2), https://www.andreaszingerle.com (6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Jahre</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>9</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>https://www.dasfundus.net (5), https://www.workstation.or.at (4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>8</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://www.anna-kraher.de (5), https://www.lllk.at (3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Projekt</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>6</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>https://www.hoerspuren.at (3), https://www.kulturviertelwochen.at (3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>5</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>https://www.okabre.com (2), https://www.totalsilence.de (3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Otto</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>4</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>https://www.otre.at (2), https://www.ottosaxinger.at (2)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: unreached_websites.csv implemented without global variable
</commit_message>
<xml_diff>
--- a/output/common_words/xls/common_words_among_websites_dict.xlsx
+++ b/output/common_words/xls/common_words_among_websites_dict.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1638,28 +1638,13 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Passwort</t>
+          <t>Otto</t>
         </is>
       </c>
       <c r="B81" t="n">
         <v>4</v>
       </c>
       <c r="C81" t="inlineStr">
-        <is>
-          <t>http://guglmugl.net (2), http://zeitgemeinschaft.at (2)</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>Otto</t>
-        </is>
-      </c>
-      <c r="B82" t="n">
-        <v>4</v>
-      </c>
-      <c r="C82" t="inlineStr">
         <is>
           <t>http://otre.at (2), http://ottosaxinger.at (2)</t>
         </is>

</xml_diff>